<commit_message>
added pictures of detection histograms for all cases
</commit_message>
<xml_diff>
--- a/Images/Test1/NLOS Measurements tables.xlsx
+++ b/Images/Test1/NLOS Measurements tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nokia-my.sharepoint.com/personal/paolo_tosi_ext_nokia_com/Documents/thesis_nlos_sensing/Images/Test1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="600" documentId="8_{1FBDE4A5-DAD5-4F82-A549-47E825905F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D37A3374-EB7E-4E6C-AC09-ACF64BCD5AB0}"/>
+  <xr:revisionPtr revIDLastSave="624" documentId="8_{1FBDE4A5-DAD5-4F82-A549-47E825905F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1252044D-D017-48DE-983F-9822A776CE69}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="5" xr2:uid="{C510919A-EA72-46EB-9FBB-3CB4D9645BFF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="5" xr2:uid="{C510919A-EA72-46EB-9FBB-3CB4D9645BFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="65">
   <si>
     <t>p_fa</t>
   </si>
@@ -1186,6 +1186,351 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>mixed_crap_ecac!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Detection rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>mixed_crap_ecac!$A$12:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>standard frame</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>standard frame + decimation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6 frames + decimation</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10 frames + decimation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>mixed_crap_ecac!$B$12:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3AAC-4A21-95D8-A68337742F96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="83953935"/>
+        <c:axId val="93954351"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="83953935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="93954351"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="93954351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="83953935"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>'Scenario 1a'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -1418,7 +1763,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4664,6 +5009,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -6497,6 +6882,511 @@
 </file>
 
 <file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -11383,15 +12273,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>272414</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>133349</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>415289</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>69532</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11411,6 +12301,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A7000C8-6A31-B514-E1E5-F3A0A4BD8F4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -12085,22 +13011,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0540B8A9-4E15-4255-A5AB-579EA55F92A0}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="22.109375" customWidth="1"/>
+    <col min="9" max="9" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12117,7 +13043,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1E-4</v>
       </c>
@@ -12131,7 +13057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
@@ -12145,7 +13071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
@@ -12162,7 +13088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>9.9999999999999995E-8</v>
       </c>
@@ -12176,7 +13102,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -12194,7 +13120,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12204,18 +13130,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D0CBF3C-8909-4785-A03F-2AECDBC477EC}">
   <dimension ref="A3:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -12223,7 +13149,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -12231,7 +13157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -12239,7 +13165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -12247,7 +13173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -12255,7 +13181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -12263,7 +13189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -12271,7 +13197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -12289,25 +13215,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6079E351-D924-45CC-9229-C7E658072511}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
-    <col min="8" max="8" width="32.140625" customWidth="1"/>
-    <col min="9" max="9" width="54.28515625" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="44.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.109375" customWidth="1"/>
+    <col min="8" max="8" width="32.109375" customWidth="1"/>
+    <col min="9" max="9" width="54.33203125" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -12345,7 +13271,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -12362,7 +13288,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -12398,7 +13324,7 @@
         <v>62.86</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -12434,7 +13360,7 @@
         <v>47.786700000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -12464,7 +13390,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -12497,7 +13423,7 @@
         <v>47.566754405014798</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -12518,7 +13444,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -12542,7 +13468,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -12578,7 +13504,7 @@
         <v>46.287999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -12605,12 +13531,12 @@
         <v>421</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>8</v>
       </c>
@@ -12630,7 +13556,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>24</v>
       </c>
@@ -12655,7 +13581,7 @@
         <v>63.574636357854871</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>27</v>
       </c>
@@ -12672,7 +13598,7 @@
         <v>46.853657778497698</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>28</v>
       </c>
@@ -12689,7 +13615,7 @@
         <v>46.616736010493199</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>31</v>
       </c>
@@ -12709,7 +13635,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E66" s="3"/>
       <c r="H66">
         <v>23</v>
@@ -12718,21 +13644,21 @@
         <v>280</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E67" s="3"/>
       <c r="H67">
         <f>H65/H66</f>
         <v>36.173913043478258</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E68" s="3"/>
       <c r="I68">
         <f>280/147</f>
         <v>1.9047619047619047</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>45</v>
       </c>
@@ -12756,7 +13682,7 @@
         <v>1.8342356237207658</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>44</v>
       </c>
@@ -12777,7 +13703,7 @@
         <v>147.60565835227234</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>47</v>
       </c>
@@ -12805,7 +13731,7 @@
         <v>1.740689518552921</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -12825,7 +13751,7 @@
         <v>0.51344086021505297</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>49</v>
       </c>
@@ -12864,16 +13790,16 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" customWidth="1"/>
+    <col min="1" max="1" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -12890,7 +13816,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -12907,7 +13833,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -12921,7 +13847,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -12935,7 +13861,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -12957,19 +13883,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69446E5-9183-4EB1-96EB-6A0DCE09238E}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -12977,7 +13903,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -12985,7 +13911,7 @@
         <v>0.6129</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -12993,7 +13919,7 @@
         <v>0.59189999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -13001,7 +13927,7 @@
         <v>0.60309999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -13009,12 +13935,52 @@
         <v>0.67569999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>64</v>
       </c>
       <c r="B6">
         <v>0.64859999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15">
+        <v>0.77</v>
       </c>
     </row>
   </sheetData>
@@ -13027,24 +13993,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C722016C-0FDB-4579-AFFB-C4A5153E0F62}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="42.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -13073,7 +14039,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -13100,7 +14066,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -13124,7 +14090,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -13151,7 +14117,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -13166,7 +14132,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -13181,7 +14147,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -13196,7 +14162,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -13211,7 +14177,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -13226,12 +14192,12 @@
         <v>896</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>8</v>
       </c>
@@ -13248,7 +14214,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -13265,7 +14231,7 @@
         <v>63.229116352035199</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -13282,7 +14248,7 @@
         <v>48.173282102770102</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -13299,7 +14265,7 @@
         <v>47.915793992282197</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -13316,12 +14282,12 @@
         <v>46.595025863529898</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H45" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>8</v>
       </c>
@@ -13341,7 +14307,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>47</v>
       </c>
@@ -13361,7 +14327,7 @@
         <v>8.2474226804123696E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -13371,7 +14337,7 @@
       <c r="C61" s="1"/>
       <c r="E61" s="3"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>49</v>
       </c>
@@ -13381,23 +14347,23 @@
       <c r="C62" s="1"/>
       <c r="E62" s="3"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C63" s="1"/>
       <c r="E63" s="3"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E64" s="3"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E65" s="3"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E66" s="3"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E67" s="3"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>50</v>
       </c>

</xml_diff>